<commit_message>
Adding gear-specific harvest outcomes by numbers and weight
</commit_message>
<xml_diff>
--- a/docs/Recruitment.xlsx
+++ b/docs/Recruitment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17910" windowHeight="13590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17910" windowHeight="13590"/>
   </bookViews>
   <sheets>
     <sheet name="Recruitment" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>SSB</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>bo</t>
   </si>
 </sst>
 </file>
@@ -946,11 +949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="421318328"/>
-        <c:axId val="503084400"/>
+        <c:axId val="506866496"/>
+        <c:axId val="506866888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="421318328"/>
+        <c:axId val="506866496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,12 +1010,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="503084400"/>
+        <c:crossAx val="506866888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="503084400"/>
+        <c:axId val="506866888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421318328"/>
+        <c:crossAx val="506866496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1974,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,14 +2521,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1">
+        <v>520000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjusted starting (equilib) conditions
</commit_message>
<xml_diff>
--- a/docs/Recruitment.xlsx
+++ b/docs/Recruitment.xlsx
@@ -949,11 +949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="506866496"/>
-        <c:axId val="506866888"/>
+        <c:axId val="256011176"/>
+        <c:axId val="256011568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="506866496"/>
+        <c:axId val="256011176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,12 +1010,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506866888"/>
+        <c:crossAx val="256011568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="506866888"/>
+        <c:axId val="256011568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506866496"/>
+        <c:crossAx val="256011176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1978,7 +1978,7 @@
   <dimension ref="A2:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>